<commit_message>
Desarrollo de carga de planilla
Se logro la carga, deserealizacion del archivo excel. Luego la lectura de los datos y el gurdado en la BD.
</commit_message>
<xml_diff>
--- a/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
+++ b/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB02\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC95D1C5-BAD4-49D8-9553-93061515678E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D4F203-39FB-4A49-82DA-2AC0570BA71E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nombres</t>
   </si>
@@ -34,24 +34,9 @@
     <t>Comentario</t>
   </si>
   <si>
-    <t>IdInstitucionFinanciera</t>
-  </si>
-  <si>
     <t>Monto</t>
   </si>
   <si>
-    <t>idDeducciones</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -68,9 +53,6 @@
   </si>
   <si>
     <t>Ahorro Personal</t>
-  </si>
-  <si>
-    <t>27</t>
   </si>
   <si>
     <t>Ramiro Alberto</t>
@@ -177,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -199,6 +181,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,24 +625,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD32D740-C6A3-4126-BE20-B91A7C0AF9FA}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -659,92 +648,71 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.78431372549019618" right="0.78431372549019618" top="0.98039215686274517" bottom="0.98039215686274517" header="0.50980392156862753" footer="0.50980392156862753"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:B4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Carga  de planilla - 85%
</commit_message>
<xml_diff>
--- a/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
+++ b/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB02\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D4F203-39FB-4A49-82DA-2AC0570BA71E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62962A9B-3A70-4D5B-BC2B-87F5799BD574}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Nombres</t>
   </si>
@@ -35,15 +35,6 @@
   </si>
   <si>
     <t>Monto</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>750</t>
-  </si>
-  <si>
-    <t>898</t>
   </si>
   <si>
     <t>cuota 1/12 - prestamo personal</t>
@@ -80,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,6 +86,18 @@
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="63"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -127,31 +130,181 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="54"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="54"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="54"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="55"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="32"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="32"/>
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="32"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="32"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -159,37 +312,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -628,91 +808,95 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <v>500.47</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="12">
+        <v>750.58</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
+      <c r="E3" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="17">
+        <v>985.24</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78431372549019618" right="0.78431372549019618" top="0.98039215686274517" bottom="0.98039215686274517" header="0.50980392156862753" footer="0.50980392156862753"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:B4" numberStoredAsText="1"/>
+    <ignoredError sqref="A4 A2 A3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revision Funcionalidad CargaDocumento - InstitucionesFinancieras
</commit_message>
<xml_diff>
--- a/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
+++ b/ERP_GMEDINA/Content/PlanillasInstitucionesFinancieras/Deduccion_Planilla_Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB02\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62962A9B-3A70-4D5B-BC2B-87F5799BD574}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DFEC8A9-455E-4944-9955-F72FE3096BE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,20 +58,20 @@
     <t>Gonzales Diaz</t>
   </si>
   <si>
-    <t>0501200008767</t>
-  </si>
-  <si>
-    <t>0501500008767</t>
-  </si>
-  <si>
-    <t>0501200808767</t>
+    <t>05012000652374</t>
+  </si>
+  <si>
+    <t>08502200036521</t>
+  </si>
+  <si>
+    <t>0502-2000-02649</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,6 +99,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -273,9 +278,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -288,9 +291,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -303,16 +304,14 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -321,6 +320,42 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,47 +365,14 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,98 +807,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD32D740-C6A3-4126-BE20-B91A7C0AF9FA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
         <v>500.47</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7">
         <v>750.58</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <v>985.24</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.78431372549019618" right="0.78431372549019618" top="0.98039215686274517" bottom="0.98039215686274517" header="0.50980392156862753" footer="0.50980392156862753"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="A4 A2 A3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>